<commit_message>
Added first steps of Functionality for choosing the group from which a user wants to see the data
</commit_message>
<xml_diff>
--- a/Documentation/DB/DB-Requests.xlsx
+++ b/Documentation/DB/DB-Requests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acs/Eigene_Dateien_Fabian/Arbeit/Studium/DHBW/Kurse/SE/BFFL/bffl/Documentation/DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2873F6C-55D4-5444-9506-713B5829652F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733F9E51-F390-2946-A3B5-B2C2EA89811E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="700" windowWidth="31500" windowHeight="18340" xr2:uid="{1A3214F4-8DD7-5C4A-BAFA-07901AA8267F}"/>
+    <workbookView xWindow="39520" yWindow="1120" windowWidth="31500" windowHeight="18340" xr2:uid="{1A3214F4-8DD7-5C4A-BAFA-07901AA8267F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1111,7 +1111,7 @@
   <dimension ref="A1:I171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Finished creating prepared statements in BE Added all endpoints in FE
</commit_message>
<xml_diff>
--- a/Documentation/DB/DB-Requests.xlsx
+++ b/Documentation/DB/DB-Requests.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acs/Eigene_Dateien_Fabian/Arbeit/Studium/DHBW/Kurse/SE/BFFL/bffl/Documentation/DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF65B1E-4B15-4440-851F-E80F52F62A14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE8BEC3-6201-B84A-AB8B-5C66329FC9B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="560" windowWidth="38320" windowHeight="20980" xr2:uid="{1A3214F4-8DD7-5C4A-BAFA-07901AA8267F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="129">
   <si>
     <t>Application area</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Detail-View-Popup, Create-Page</t>
-  </si>
-  <si>
-    <t>/api/assignTagById</t>
   </si>
   <si>
     <t>Assign one Tag of a group to a ShortURL from that group</t>
@@ -190,9 +187,6 @@
     <t>Delete ShortURL</t>
   </si>
   <si>
-    <t>/api/deleteShortURLByID</t>
-  </si>
-  <si>
     <t>Delete Tag</t>
   </si>
   <si>
@@ -205,9 +199,6 @@
     <t>Group-Menu</t>
   </si>
   <si>
-    <t>/api/deleteTagByID</t>
-  </si>
-  <si>
     <t>searched_tag_id</t>
   </si>
   <si>
@@ -238,45 +229,21 @@
     <t>/api/deleteGroup</t>
   </si>
   <si>
-    <t>Add a new user to a given group with limit</t>
-  </si>
-  <si>
     <t>/api/addUserToGroup</t>
   </si>
   <si>
     <t>searched_group_name, new_user_id, new_end_timestamp</t>
   </si>
   <si>
-    <t>Add a new user to a given group without limit</t>
-  </si>
-  <si>
-    <t>searched_group_name, new_user_id</t>
-  </si>
-  <si>
-    <t>Add a new user with admin status to a given group with limit</t>
-  </si>
-  <si>
-    <t>Add a new user  with admin status to a given group without limit</t>
-  </si>
-  <si>
-    <t>/api/addAdminToGroup</t>
-  </si>
-  <si>
     <t>searched_group_name, groupmember_user_id, new_user_id, new_end_timestamp</t>
   </si>
   <si>
-    <t>searched_group_name, groupmember_user_id, new_user_id</t>
-  </si>
-  <si>
     <t>Update admin status for given user in given group</t>
   </si>
   <si>
     <t>Update limit for membership of given user in given group</t>
   </si>
   <si>
-    <t>/api/updateUserState</t>
-  </si>
-  <si>
     <t>searched_user_id, groupmember_user_id, searched_group_name, new_admin_flag</t>
   </si>
   <si>
@@ -304,19 +271,10 @@
     <t>/s/${searched_group_id}/ ${searched_custom_suffix}</t>
   </si>
   <si>
-    <t>searched_group_id, searched_custom_suffix</t>
-  </si>
-  <si>
     <t>Register Usage of a ShortURL with region</t>
   </si>
   <si>
-    <t>searched_short_url_id, new_client_ip, new_region</t>
-  </si>
-  <si>
     <t>Register Usage of a ShortURL without region</t>
-  </si>
-  <si>
-    <t>searched_short_url_id, new_client_ip</t>
   </si>
   <si>
     <t>x</t>
@@ -363,9 +321,6 @@
 WHERE group_name = ( SELECT group_name FROM short_url WHERE id = :searched_short_url_id) AND id = :chosen_tag_id));</t>
   </si>
   <si>
-    <t>UPDATE short_url SET custom_suffix = :new_custom_suffix WHERE custom_suffix != :new_custom_suffix AND id = :searched_short_url_id AND update_flag = true;</t>
-  </si>
-  <si>
     <t>UPDATE short_url SET scope = :new_scope WHERE CURRENT_TIMESTAMP + 3600 * interval '1 second' &lt; (( SELECT create_timestamp FROM short_url WHERE id = :searched_short_url_id) + :new_scope * interval '1 second') AND scope != :new_scope AND id = :searched_short_url_id AND update_flag = true;</t>
   </si>
   <si>
@@ -409,15 +364,9 @@
     <t>INSERT into user_has_group (user_id, group_name, start_timestamp, end_timestamp) VALUES (:new_user_id, :searched_group_name, CURRENT_TIMESTAMP, :new_end_timestamp);</t>
   </si>
   <si>
-    <t>INSERT into user_has_group (user_id, group_name, start_timestamp, end_timestamp) VALUES (:new_user_id, :searched_group_name, CURRENT_TIMESTAMP, NULL);</t>
-  </si>
-  <si>
     <t>INSERT INTO user_has_group (user_id, group_name, start_timestamp, end_timestamp, admin_flag) VALUES (:new_user_id, ( SELECT G.name FROM app_group_g, user_has_group UhG WHERE UhG.group_name = G.name AND G.name = :searched_group_name AND UhG.user_id = :groupmember_user_id AND UhG.admin_flag = true ), CURRENT_TIMESTAMP, :new_end_timestamp, true);</t>
   </si>
   <si>
-    <t>INSERT INTO user_has_group (user_id, group_name, start_timestamp, end_timestamp, admin_flag) VALUES (:new_user_id, ( SELECT G.name FROM app_group_g, user_has_group UhG WHERE UhG.group_name = G.name AND G.name = :searched_group_name AND UhG.user_id = :groupmember_user_id AND UhG.admin_flag = true ), CURRENT_TIMESTAMP, NULL, true);</t>
-  </si>
-  <si>
     <t>UPDATE user_has_group SET admin_flag = :new_admin_flag  WHERE user_id = :searched_user_id AND group_name = ( SELECT group_name FROM user_has_group WHERE user_id = :groupmember_user_id AND admin_flag = true AND group_name = :searched_group_name );</t>
   </si>
   <si>
@@ -430,13 +379,55 @@
     <t>SELECT T.url FROM assigned_target T WHERE T.short_url_id = ( SELECT id FROM short_url WHERE group_name = :searched_group_name AND custom_suffix = :searched_custom_suffix ) AND assign_timestamp = ( SELECT MAX(assign_timestamp) FROM assigned_target  WHERE short_url_id = T.short_url_id GROUP BY short_url_id );</t>
   </si>
   <si>
-    <t>INSERT INTO url_call (client_ip, short_url_id, call_timestamp, region) VALUES (:new_client_ip, :searched_short_url_id, CURRENT_TIMESTAMP, :new_region);</t>
-  </si>
-  <si>
-    <t>INSERT INTO url_call (client_ip, short_url_id, call_timestamp) VALUES (:new_client_ip, :searched_short_url_id, CURRENT_TIMESTAMP);</t>
-  </si>
-  <si>
     <t>/api/createShortURLFor GroupWithOptionalTags</t>
+  </si>
+  <si>
+    <t>UPDATE short_url SET custom_suffix = :new_custom_suffix WHERE id = :searched_short_url_id AND custom_suffix != :new_custom_suffix AND update_flag = true;</t>
+  </si>
+  <si>
+    <t>/api/assignTagToShortURLById</t>
+  </si>
+  <si>
+    <t>/api/deleteTag</t>
+  </si>
+  <si>
+    <t>/api/deleteShortURL</t>
+  </si>
+  <si>
+    <t>/api/addUserAsAdminToGroup</t>
+  </si>
+  <si>
+    <t>Add a new user with admin status to a given group</t>
+  </si>
+  <si>
+    <t>Add a new user to a given group</t>
+  </si>
+  <si>
+    <t>/api/updateAdminStateOfUser</t>
+  </si>
+  <si>
+    <t>Get all Calls of a certain ShortURL with Target</t>
+  </si>
+  <si>
+    <t>searched_group_name, searched_custom_suffix</t>
+  </si>
+  <si>
+    <t>searched_group_name, searched_custom_suffix, new_client_ip, new_region</t>
+  </si>
+  <si>
+    <t>INSERT INTO url_call (client_ip, short_url_id, call_timestamp, region) VALUES (:new_client_ip, ( SELECT id FROM short_url WHERE group_name = :searched_group_name AND custom_suffix = :searched_custom_suffix ), CURRENT_TIMESTAMP, :new_region);</t>
+  </si>
+  <si>
+    <t>searched_group_name, searched_custom_suffix, new_client_ip</t>
+  </si>
+  <si>
+    <t>INSERT INTO url_call (client_ip, short_url_id, call_timestamp) VALUES (:new_client_ip, ( SELECT id FROM short_url WHERE group_name = :searched_group_name AND custom_suffix = :searched_custom_suffix ), CURRENT_TIMESTAMP);</t>
+  </si>
+  <si>
+    <t>/api/callsOfShortURL</t>
+  </si>
+  <si>
+    <t>SELECT C.client_ip, S.group_name, S.custom_suffix, T.url, C.call_timestamp FROM url_call C INNER JOIN short_url S ON C.short_url_id = S.id  INNER JOIN assigned_target T ON S.id = T.short_url_id WHERE S.id = 1 AND T.assign_timestamp = ( SELECT assign_timestamp FROM assigned_target WHERE short_url_id = S.id AND assign_timestamp &lt;= C.call_timestamp ORDER BY assign_timestamp DESC LIMIT 1 );</t>
   </si>
 </sst>
 </file>
@@ -466,7 +457,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,19 +484,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5C8D5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -625,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -747,32 +726,20 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -782,9 +749,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1106,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DAB8FD-6609-A543-99E3-1E0DA2A4E869}">
-  <dimension ref="A1:J171"/>
+  <dimension ref="A1:J169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1132,15 +1096,15 @@
       <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="52"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="48"/>
     </row>
     <row r="3" spans="1:10" ht="34" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -1186,11 +1150,11 @@
         <v>14</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="31" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.2">
@@ -1204,7 +1168,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>8</v>
@@ -1213,10 +1177,10 @@
         <v>12</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="130" customHeight="1" x14ac:dyDescent="0.2">
@@ -1239,10 +1203,10 @@
         <v>19</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="56" customHeight="1" x14ac:dyDescent="0.2">
@@ -1256,7 +1220,7 @@
         <v>25</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>8</v>
@@ -1265,10 +1229,10 @@
         <v>19</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
@@ -1291,10 +1255,10 @@
         <v>12</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="52" customHeight="1" x14ac:dyDescent="0.2">
@@ -1302,13 +1266,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>8</v>
@@ -1317,10 +1281,10 @@
         <v>19</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="204" customHeight="1" x14ac:dyDescent="0.2">
@@ -1333,20 +1297,20 @@
       <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="53" t="s">
-        <v>131</v>
+      <c r="E10" s="45" t="s">
+        <v>112</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="98" customHeight="1" x14ac:dyDescent="0.2">
@@ -1354,25 +1318,25 @@
         <v>8</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>106</v>
+        <v>28</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.2">
@@ -1380,22 +1344,25 @@
         <v>9</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="34" t="s">
         <v>30</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>31</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>107</v>
+        <v>113</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="98" customHeight="1" x14ac:dyDescent="0.2">
@@ -1403,22 +1370,25 @@
         <v>10</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="34" t="s">
         <v>30</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>31</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>108</v>
+        <v>93</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.2">
@@ -1426,22 +1396,25 @@
         <v>11</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="34" t="s">
         <v>30</v>
-      </c>
-      <c r="E14" s="34" t="s">
-        <v>31</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>109</v>
+        <v>94</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.2">
@@ -1449,22 +1422,25 @@
         <v>12</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="34" t="s">
         <v>30</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>31</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>110</v>
+        <v>95</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.2">
@@ -1472,151 +1448,169 @@
         <v>13</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="34" t="s">
         <v>30</v>
-      </c>
-      <c r="E16" s="34" t="s">
-        <v>31</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="37">
         <v>14</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="35">
         <v>15</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="36">
         <v>16</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="25">
         <v>17</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="13">
         <v>18</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="9">
         <v>19</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D22" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>8</v>
@@ -1625,309 +1619,333 @@
         <v>19</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="25">
         <v>20</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="13">
         <v>21</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>62</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="9">
         <v>22</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G25" s="21" t="s">
         <v>12</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="43">
+        <v>105</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="25">
         <v>23</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="40" t="s">
-        <v>68</v>
+        <v>53</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="40">
+        <v>106</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="115" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="9">
         <v>24</v>
       </c>
-      <c r="C27" s="18" t="s">
-        <v>70</v>
+      <c r="C27" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>68</v>
+        <v>53</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="115" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="47">
+        <v>107</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="13">
         <v>25</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>72</v>
+      <c r="C28" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="46" t="s">
-        <v>74</v>
+        <v>53</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="48">
+        <v>108</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="9">
         <v>26</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>73</v>
+      <c r="C29" s="16" t="s">
+        <v>68</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29" s="46" t="s">
-        <v>74</v>
+        <v>53</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="78" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="13">
+        <v>109</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="25">
         <v>27</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G30" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H30" s="20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="9">
+    </row>
+    <row r="31" spans="2:10" ht="98" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="40">
         <v>28</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="42">
+        <v>29</v>
+      </c>
+      <c r="C32" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="H31" s="20" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="78" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="25">
-        <v>29</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>83</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
+      </c>
+      <c r="E32" s="43" t="s">
+        <v>77</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="H32" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="44">
+        <v>30</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="13">
+        <v>31</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="41">
-        <v>30</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E33" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="F33" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="H33" s="20" t="s">
+      <c r="G34" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="20" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="44">
-        <v>31</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="H34" s="20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="49">
+    <row r="35" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="9">
         <v>32</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E35" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="16"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="20"/>
+    </row>
+    <row r="36" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="13">
         <v>33</v>
       </c>
@@ -1938,30 +1956,30 @@
       <c r="G36" s="21"/>
       <c r="H36" s="20"/>
     </row>
-    <row r="37" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="9">
         <v>34</v>
       </c>
-      <c r="C37" s="16"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="21"/>
       <c r="H37" s="20"/>
     </row>
-    <row r="38" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="25">
+    <row r="38" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="13">
         <v>35</v>
       </c>
-      <c r="C38" s="18"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="21"/>
       <c r="H38" s="20"/>
     </row>
-    <row r="39" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="13">
+    <row r="39" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="9">
         <v>36</v>
       </c>
       <c r="C39" s="18"/>
@@ -1971,29 +1989,29 @@
       <c r="G39" s="21"/>
       <c r="H39" s="20"/>
     </row>
-    <row r="40" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="9">
+    <row r="40" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="13">
         <v>37</v>
       </c>
-      <c r="C40" s="16"/>
+      <c r="C40" s="18"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="21"/>
       <c r="H40" s="20"/>
     </row>
-    <row r="41" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="25">
+    <row r="41" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="9">
         <v>38</v>
       </c>
-      <c r="C41" s="18"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="21"/>
       <c r="H41" s="20"/>
     </row>
-    <row r="42" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="13">
         <v>39</v>
       </c>
@@ -2004,30 +2022,30 @@
       <c r="G42" s="21"/>
       <c r="H42" s="20"/>
     </row>
-    <row r="43" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="9">
         <v>40</v>
       </c>
-      <c r="C43" s="16"/>
+      <c r="C43" s="18"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="21"/>
       <c r="H43" s="20"/>
     </row>
-    <row r="44" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="25">
+    <row r="44" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="13">
         <v>41</v>
       </c>
-      <c r="C44" s="18"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="21"/>
       <c r="H44" s="20"/>
     </row>
-    <row r="45" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="13">
+    <row r="45" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="9">
         <v>42</v>
       </c>
       <c r="C45" s="18"/>
@@ -2037,29 +2055,29 @@
       <c r="G45" s="21"/>
       <c r="H45" s="20"/>
     </row>
-    <row r="46" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="9">
+    <row r="46" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="13">
         <v>43</v>
       </c>
-      <c r="C46" s="16"/>
+      <c r="C46" s="18"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="21"/>
       <c r="H46" s="20"/>
     </row>
-    <row r="47" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="25">
+    <row r="47" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="9">
         <v>44</v>
       </c>
-      <c r="C47" s="18"/>
+      <c r="C47" s="16"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="21"/>
       <c r="H47" s="20"/>
     </row>
-    <row r="48" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="13">
         <v>45</v>
       </c>
@@ -2074,7 +2092,7 @@
       <c r="B49" s="9">
         <v>46</v>
       </c>
-      <c r="C49" s="16"/>
+      <c r="C49" s="18"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -2082,10 +2100,10 @@
       <c r="H49" s="20"/>
     </row>
     <row r="50" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="25">
+      <c r="B50" s="13">
         <v>47</v>
       </c>
-      <c r="C50" s="18"/>
+      <c r="C50" s="16"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -2093,7 +2111,7 @@
       <c r="H50" s="20"/>
     </row>
     <row r="51" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="13">
+      <c r="B51" s="9">
         <v>48</v>
       </c>
       <c r="C51" s="18"/>
@@ -2104,10 +2122,10 @@
       <c r="H51" s="20"/>
     </row>
     <row r="52" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="9">
+      <c r="B52" s="13">
         <v>49</v>
       </c>
-      <c r="C52" s="16"/>
+      <c r="C52" s="18"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -2115,10 +2133,10 @@
       <c r="H52" s="20"/>
     </row>
     <row r="53" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="25">
+      <c r="B53" s="9">
         <v>50</v>
       </c>
-      <c r="C53" s="18"/>
+      <c r="C53" s="16"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -2140,7 +2158,7 @@
       <c r="B55" s="9">
         <v>52</v>
       </c>
-      <c r="C55" s="16"/>
+      <c r="C55" s="18"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -2148,10 +2166,10 @@
       <c r="H55" s="20"/>
     </row>
     <row r="56" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="25">
+      <c r="B56" s="13">
         <v>53</v>
       </c>
-      <c r="C56" s="18"/>
+      <c r="C56" s="16"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -2159,7 +2177,7 @@
       <c r="H56" s="20"/>
     </row>
     <row r="57" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="13">
+      <c r="B57" s="9">
         <v>54</v>
       </c>
       <c r="C57" s="18"/>
@@ -2170,10 +2188,10 @@
       <c r="H57" s="20"/>
     </row>
     <row r="58" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="9">
+      <c r="B58" s="13">
         <v>55</v>
       </c>
-      <c r="C58" s="16"/>
+      <c r="C58" s="18"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -2181,10 +2199,10 @@
       <c r="H58" s="20"/>
     </row>
     <row r="59" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="25">
+      <c r="B59" s="9">
         <v>56</v>
       </c>
-      <c r="C59" s="18"/>
+      <c r="C59" s="16"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -2206,7 +2224,7 @@
       <c r="B61" s="9">
         <v>58</v>
       </c>
-      <c r="C61" s="16"/>
+      <c r="C61" s="18"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -2214,10 +2232,10 @@
       <c r="H61" s="20"/>
     </row>
     <row r="62" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="25">
+      <c r="B62" s="13">
         <v>59</v>
       </c>
-      <c r="C62" s="18"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -2225,7 +2243,7 @@
       <c r="H62" s="20"/>
     </row>
     <row r="63" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="13">
+      <c r="B63" s="9">
         <v>60</v>
       </c>
       <c r="C63" s="18"/>
@@ -2236,10 +2254,10 @@
       <c r="H63" s="20"/>
     </row>
     <row r="64" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="9">
+      <c r="B64" s="13">
         <v>61</v>
       </c>
-      <c r="C64" s="16"/>
+      <c r="C64" s="18"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -2247,10 +2265,10 @@
       <c r="H64" s="20"/>
     </row>
     <row r="65" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="25">
+      <c r="B65" s="9">
         <v>62</v>
       </c>
-      <c r="C65" s="18"/>
+      <c r="C65" s="16"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -2272,7 +2290,7 @@
       <c r="B67" s="9">
         <v>64</v>
       </c>
-      <c r="C67" s="16"/>
+      <c r="C67" s="18"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -2280,10 +2298,10 @@
       <c r="H67" s="20"/>
     </row>
     <row r="68" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="25">
+      <c r="B68" s="13">
         <v>65</v>
       </c>
-      <c r="C68" s="18"/>
+      <c r="C68" s="16"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
@@ -2291,7 +2309,7 @@
       <c r="H68" s="20"/>
     </row>
     <row r="69" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="13">
+      <c r="B69" s="9">
         <v>66</v>
       </c>
       <c r="C69" s="18"/>
@@ -2302,10 +2320,10 @@
       <c r="H69" s="20"/>
     </row>
     <row r="70" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="9">
+      <c r="B70" s="13">
         <v>67</v>
       </c>
-      <c r="C70" s="16"/>
+      <c r="C70" s="18"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -2313,10 +2331,10 @@
       <c r="H70" s="20"/>
     </row>
     <row r="71" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="25">
+      <c r="B71" s="9">
         <v>68</v>
       </c>
-      <c r="C71" s="18"/>
+      <c r="C71" s="33"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
@@ -2327,7 +2345,7 @@
       <c r="B72" s="13">
         <v>69</v>
       </c>
-      <c r="C72" s="18"/>
+      <c r="C72" s="19"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -2338,7 +2356,7 @@
       <c r="B73" s="9">
         <v>70</v>
       </c>
-      <c r="C73" s="33"/>
+      <c r="C73" s="19"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -2346,7 +2364,7 @@
       <c r="H73" s="20"/>
     </row>
     <row r="74" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="25">
+      <c r="B74" s="13">
         <v>71</v>
       </c>
       <c r="C74" s="19"/>
@@ -2357,7 +2375,7 @@
       <c r="H74" s="20"/>
     </row>
     <row r="75" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="13">
+      <c r="B75" s="9">
         <v>72</v>
       </c>
       <c r="C75" s="19"/>
@@ -2369,7 +2387,7 @@
     </row>
     <row r="76" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="13">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C76" s="19"/>
       <c r="D76" s="3"/>
@@ -2379,8 +2397,8 @@
       <c r="H76" s="20"/>
     </row>
     <row r="77" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="13">
-        <v>73</v>
+      <c r="B77" s="9">
+        <v>74</v>
       </c>
       <c r="C77" s="19"/>
       <c r="D77" s="3"/>
@@ -2391,7 +2409,7 @@
     </row>
     <row r="78" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="13">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C78" s="19"/>
       <c r="D78" s="3"/>
@@ -2401,8 +2419,8 @@
       <c r="H78" s="20"/>
     </row>
     <row r="79" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="13">
-        <v>75</v>
+      <c r="B79" s="9">
+        <v>76</v>
       </c>
       <c r="C79" s="19"/>
       <c r="D79" s="3"/>
@@ -2413,9 +2431,9 @@
     </row>
     <row r="80" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="13">
-        <v>76</v>
-      </c>
-      <c r="C80" s="19"/>
+        <v>77</v>
+      </c>
+      <c r="C80" s="12"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
@@ -2423,10 +2441,10 @@
       <c r="H80" s="20"/>
     </row>
     <row r="81" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="13">
-        <v>77</v>
-      </c>
-      <c r="C81" s="19"/>
+      <c r="B81" s="9">
+        <v>78</v>
+      </c>
+      <c r="C81" s="12"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
@@ -2435,7 +2453,7 @@
     </row>
     <row r="82" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="13">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C82" s="12"/>
       <c r="D82" s="3"/>
@@ -2445,37 +2463,33 @@
       <c r="H82" s="20"/>
     </row>
     <row r="83" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="13">
-        <v>79</v>
+      <c r="B83" s="9">
+        <v>80</v>
       </c>
       <c r="C83" s="12"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
-      <c r="G83" s="21"/>
+      <c r="G83" s="3"/>
       <c r="H83" s="20"/>
     </row>
     <row r="84" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B84" s="13">
-        <v>80</v>
-      </c>
+      <c r="B84" s="13"/>
       <c r="C84" s="12"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
-      <c r="G84" s="21"/>
+      <c r="G84" s="3"/>
       <c r="H84" s="20"/>
     </row>
     <row r="85" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B85" s="13">
-        <v>81</v>
-      </c>
+      <c r="B85" s="13"/>
       <c r="C85" s="12"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
-      <c r="H85" s="20"/>
+      <c r="H85" s="16"/>
     </row>
     <row r="86" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="13"/>
@@ -2484,7 +2498,7 @@
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
-      <c r="H86" s="20"/>
+      <c r="H86" s="16"/>
     </row>
     <row r="87" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="13"/>
@@ -3152,50 +3166,32 @@
       <c r="G160" s="3"/>
       <c r="H160" s="16"/>
     </row>
-    <row r="161" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" s="13"/>
-      <c r="C161" s="12"/>
-      <c r="D161" s="3"/>
-      <c r="E161" s="3"/>
-      <c r="F161" s="3"/>
-      <c r="G161" s="3"/>
-      <c r="H161" s="16"/>
-    </row>
-    <row r="162" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="162" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B162" s="13"/>
-      <c r="C162" s="12"/>
-      <c r="D162" s="3"/>
-      <c r="E162" s="3"/>
-      <c r="F162" s="3"/>
-      <c r="G162" s="3"/>
-      <c r="H162" s="16"/>
-    </row>
-    <row r="163" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="163" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B163" s="13"/>
     </row>
-    <row r="164" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B164" s="13"/>
     </row>
-    <row r="165" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B165" s="13"/>
     </row>
-    <row r="166" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B166" s="13"/>
     </row>
-    <row r="167" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B167" s="13"/>
     </row>
-    <row r="168" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B168" s="13"/>
     </row>
-    <row r="169" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B169" s="13"/>
-    </row>
-    <row r="170" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B170" s="13"/>
-    </row>
-    <row r="171" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B171" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>